<commit_message>
Filtrage jour et semaines vides.
</commit_message>
<xml_diff>
--- a/all.xlsx
+++ b/all.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1381" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1380" uniqueCount="107">
   <si>
     <t xml:space="preserve">Semaine : </t>
   </si>
@@ -379,7 +379,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:I353"/>
+  <dimension ref="A1:I352"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -4827,36 +4827,51 @@
     </row>
     <row r="231">
       <c r="A231" t="n" s="1">
-        <v>45972.0</v>
+        <v>45973.0</v>
       </c>
       <c r="B231" t="s" s="0">
-        <v>18</v>
+        <v>23</v>
       </c>
     </row>
     <row r="232">
-      <c r="A232" t="n" s="1">
-        <v>45973.0</v>
-      </c>
-      <c r="B232" t="s" s="0">
-        <v>23</v>
-      </c>
+      <c r="A232" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B232" s="0"/>
+      <c r="C232" s="0"/>
+      <c r="D232" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E232" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="F232" s="0"/>
+      <c r="G232" s="0"/>
+      <c r="H232" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="I232" s="0"/>
     </row>
     <row r="233">
       <c r="A233" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="B233" s="0"/>
-      <c r="C233" s="0"/>
+        <v>83</v>
+      </c>
+      <c r="B233" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="C233" t="s" s="0">
+        <v>75</v>
+      </c>
       <c r="D233" t="s" s="0">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E233" t="n" s="0">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="F233" s="0"/>
       <c r="G233" s="0"/>
       <c r="H233" t="s" s="0">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="I233" s="0"/>
     </row>
@@ -4871,7 +4886,7 @@
         <v>75</v>
       </c>
       <c r="D234" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E234" t="n" s="0">
         <v>2.0</v>
@@ -4884,79 +4899,79 @@
       <c r="I234" s="0"/>
     </row>
     <row r="235">
-      <c r="A235" t="s" s="0">
-        <v>83</v>
+      <c r="A235" t="n" s="1">
+        <v>45974.0</v>
       </c>
       <c r="B235" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="C235" t="s" s="0">
-        <v>75</v>
-      </c>
-      <c r="D235" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E235" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F235" s="0"/>
-      <c r="G235" s="0"/>
-      <c r="H235" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="I235" s="0"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="236">
-      <c r="A236" t="n" s="1">
-        <v>45974.0</v>
+      <c r="A236" t="s" s="0">
+        <v>66</v>
       </c>
       <c r="B236" t="s" s="0">
-        <v>27</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="C236" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D236" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E236" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="F236" s="0"/>
+      <c r="G236" s="0"/>
+      <c r="H236" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="I236" s="0"/>
     </row>
     <row r="237">
-      <c r="A237" t="s" s="0">
-        <v>66</v>
+      <c r="A237" t="n" s="1">
+        <v>45975.0</v>
       </c>
       <c r="B237" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="C237" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D237" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E237" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="F237" s="0"/>
-      <c r="G237" s="0"/>
-      <c r="H237" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="I237" s="0"/>
+        <v>34</v>
+      </c>
     </row>
     <row r="238">
-      <c r="A238" t="n" s="1">
-        <v>45975.0</v>
+      <c r="A238" t="s" s="0">
+        <v>59</v>
       </c>
       <c r="B238" t="s" s="0">
-        <v>34</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C238" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="D238" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E238" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F238" s="0"/>
+      <c r="G238" s="0"/>
+      <c r="H238" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="I238" s="0"/>
     </row>
     <row r="239">
       <c r="A239" t="s" s="0">
-        <v>59</v>
+        <v>84</v>
       </c>
       <c r="B239" t="s" s="0">
-        <v>60</v>
+        <v>12</v>
       </c>
       <c r="C239" t="s" s="0">
-        <v>61</v>
+        <v>85</v>
       </c>
       <c r="D239" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E239" t="n" s="0">
         <v>2.0</v>
@@ -4964,48 +4979,50 @@
       <c r="F239" s="0"/>
       <c r="G239" s="0"/>
       <c r="H239" t="s" s="0">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="I239" s="0"/>
     </row>
     <row r="240">
       <c r="A240" t="s" s="0">
-        <v>84</v>
-      </c>
-      <c r="B240" t="s" s="0">
-        <v>12</v>
-      </c>
-      <c r="C240" t="s" s="0">
-        <v>85</v>
-      </c>
-      <c r="D240" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E240" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F240" s="0"/>
-      <c r="G240" s="0"/>
-      <c r="H240" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="I240" s="0"/>
+        <v>0</v>
+      </c>
+      <c r="B240" t="n" s="0">
+        <v>47.0</v>
+      </c>
     </row>
     <row r="241">
-      <c r="A241" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B241" t="n" s="0">
-        <v>47.0</v>
+      <c r="A241" t="n" s="1">
+        <v>45978.0</v>
+      </c>
+      <c r="B241" t="s" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="242">
-      <c r="A242" t="n" s="1">
-        <v>45978.0</v>
+      <c r="A242" t="s" s="0">
+        <v>48</v>
       </c>
       <c r="B242" t="s" s="0">
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C242" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D242" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E242" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F242" s="0"/>
+      <c r="G242" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="H242" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="I242" s="0"/>
     </row>
     <row r="243">
       <c r="A243" t="s" s="0">
@@ -5018,14 +5035,14 @@
         <v>8</v>
       </c>
       <c r="D243" t="s" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E243" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F243" s="0"/>
       <c r="G243" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H243" t="s" s="0">
         <v>32</v>
@@ -5034,41 +5051,39 @@
     </row>
     <row r="244">
       <c r="A244" t="s" s="0">
-        <v>48</v>
+        <v>20</v>
       </c>
       <c r="B244" t="s" s="0">
-        <v>7</v>
+        <v>21</v>
       </c>
       <c r="C244" t="s" s="0">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="D244" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E244" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F244" s="0"/>
-      <c r="G244" t="s" s="0">
-        <v>33</v>
-      </c>
+      <c r="G244" s="0"/>
       <c r="H244" t="s" s="0">
-        <v>32</v>
+        <v>10</v>
       </c>
       <c r="I244" s="0"/>
     </row>
     <row r="245">
       <c r="A245" t="s" s="0">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="B245" t="s" s="0">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="C245" t="s" s="0">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="D245" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E245" t="n" s="0">
         <v>2.0</v>
@@ -5082,59 +5097,59 @@
     </row>
     <row r="246">
       <c r="A246" t="s" s="0">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B246" t="s" s="0">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="C246" t="s" s="0">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D246" t="s" s="0">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E246" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F246" s="0"/>
-      <c r="G246" s="0"/>
+      <c r="G246" t="s" s="0">
+        <v>33</v>
+      </c>
       <c r="H246" t="s" s="0">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="I246" s="0"/>
     </row>
     <row r="247">
-      <c r="A247" t="s" s="0">
-        <v>69</v>
+      <c r="A247" t="n" s="1">
+        <v>45979.0</v>
       </c>
       <c r="B247" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="C247" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="D247" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E247" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F247" s="0"/>
-      <c r="G247" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="H247" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="I247" s="0"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="248">
-      <c r="A248" t="n" s="1">
-        <v>45979.0</v>
+      <c r="A248" t="s" s="0">
+        <v>79</v>
       </c>
       <c r="B248" t="s" s="0">
-        <v>18</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C248" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="D248" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E248" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F248" s="0"/>
+      <c r="G248" s="0"/>
+      <c r="H248" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="I248" s="0"/>
     </row>
     <row r="249">
       <c r="A249" t="s" s="0">
@@ -5147,7 +5162,7 @@
         <v>82</v>
       </c>
       <c r="D249" t="s" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E249" t="n" s="0">
         <v>2.0</v>
@@ -5160,98 +5175,98 @@
       <c r="I249" s="0"/>
     </row>
     <row r="250">
-      <c r="A250" t="s" s="0">
-        <v>79</v>
+      <c r="A250" t="n" s="1">
+        <v>45980.0</v>
       </c>
       <c r="B250" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C250" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="D250" t="s" s="0">
-        <v>9</v>
-      </c>
-      <c r="E250" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F250" s="0"/>
-      <c r="G250" s="0"/>
-      <c r="H250" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="I250" s="0"/>
+        <v>23</v>
+      </c>
     </row>
     <row r="251">
-      <c r="A251" t="n" s="1">
-        <v>45980.0</v>
-      </c>
-      <c r="B251" t="s" s="0">
-        <v>23</v>
-      </c>
+      <c r="A251" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B251" s="0"/>
+      <c r="C251" s="0"/>
+      <c r="D251" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E251" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="F251" s="0"/>
+      <c r="G251" s="0"/>
+      <c r="H251" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="I251" s="0"/>
     </row>
     <row r="252">
       <c r="A252" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="B252" s="0"/>
-      <c r="C252" s="0"/>
+        <v>67</v>
+      </c>
+      <c r="B252" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C252" t="s" s="0">
+        <v>68</v>
+      </c>
       <c r="D252" t="s" s="0">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E252" t="n" s="0">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="F252" s="0"/>
       <c r="G252" s="0"/>
       <c r="H252" t="s" s="0">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I252" s="0"/>
     </row>
     <row r="253">
-      <c r="A253" t="s" s="0">
-        <v>67</v>
+      <c r="A253" t="n" s="1">
+        <v>45981.0</v>
       </c>
       <c r="B253" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="C253" t="s" s="0">
-        <v>68</v>
-      </c>
-      <c r="D253" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E253" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F253" s="0"/>
-      <c r="G253" s="0"/>
-      <c r="H253" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="I253" s="0"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="254">
-      <c r="A254" t="n" s="1">
-        <v>45981.0</v>
+      <c r="A254" t="s" s="0">
+        <v>84</v>
       </c>
       <c r="B254" t="s" s="0">
-        <v>27</v>
-      </c>
+        <v>12</v>
+      </c>
+      <c r="C254" t="s" s="0">
+        <v>13</v>
+      </c>
+      <c r="D254" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E254" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F254" s="0"/>
+      <c r="G254" s="0"/>
+      <c r="H254" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="I254" s="0"/>
     </row>
     <row r="255">
       <c r="A255" t="s" s="0">
-        <v>84</v>
+        <v>20</v>
       </c>
       <c r="B255" t="s" s="0">
-        <v>12</v>
+        <v>21</v>
       </c>
       <c r="C255" t="s" s="0">
-        <v>13</v>
+        <v>22</v>
       </c>
       <c r="D255" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E255" t="n" s="0">
         <v>2.0</v>
@@ -5259,22 +5274,22 @@
       <c r="F255" s="0"/>
       <c r="G255" s="0"/>
       <c r="H255" t="s" s="0">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="I255" s="0"/>
     </row>
     <row r="256">
       <c r="A256" t="s" s="0">
-        <v>20</v>
+        <v>67</v>
       </c>
       <c r="B256" t="s" s="0">
-        <v>21</v>
+        <v>60</v>
       </c>
       <c r="C256" t="s" s="0">
-        <v>22</v>
+        <v>68</v>
       </c>
       <c r="D256" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E256" t="n" s="0">
         <v>2.0</v>
@@ -5288,59 +5303,59 @@
     </row>
     <row r="257">
       <c r="A257" t="s" s="0">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="B257" t="s" s="0">
-        <v>60</v>
+        <v>21</v>
       </c>
       <c r="C257" t="s" s="0">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="D257" t="s" s="0">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E257" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F257" s="0"/>
-      <c r="G257" s="0"/>
+      <c r="G257" t="s" s="0">
+        <v>31</v>
+      </c>
       <c r="H257" t="s" s="0">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="I257" s="0"/>
     </row>
     <row r="258">
-      <c r="A258" t="s" s="0">
-        <v>69</v>
+      <c r="A258" t="n" s="1">
+        <v>45982.0</v>
       </c>
       <c r="B258" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="C258" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="D258" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E258" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F258" s="0"/>
-      <c r="G258" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="H258" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="I258" s="0"/>
+        <v>34</v>
+      </c>
     </row>
     <row r="259">
-      <c r="A259" t="n" s="1">
-        <v>45982.0</v>
+      <c r="A259" t="s" s="0">
+        <v>83</v>
       </c>
       <c r="B259" t="s" s="0">
-        <v>34</v>
-      </c>
+        <v>45</v>
+      </c>
+      <c r="C259" t="s" s="0">
+        <v>75</v>
+      </c>
+      <c r="D259" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E259" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F259" s="0"/>
+      <c r="G259" s="0"/>
+      <c r="H259" t="s" s="0">
+        <v>39</v>
+      </c>
+      <c r="I259" s="0"/>
     </row>
     <row r="260">
       <c r="A260" t="s" s="0">
@@ -5353,7 +5368,7 @@
         <v>75</v>
       </c>
       <c r="D260" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E260" t="n" s="0">
         <v>2.0</v>
@@ -5367,16 +5382,16 @@
     </row>
     <row r="261">
       <c r="A261" t="s" s="0">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="B261" t="s" s="0">
-        <v>45</v>
+        <v>53</v>
       </c>
       <c r="C261" t="s" s="0">
-        <v>75</v>
+        <v>65</v>
       </c>
       <c r="D261" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E261" t="n" s="0">
         <v>2.0</v>
@@ -5390,42 +5405,38 @@
     </row>
     <row r="262">
       <c r="A262" t="s" s="0">
-        <v>86</v>
-      </c>
-      <c r="B262" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="C262" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="D262" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E262" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F262" s="0"/>
-      <c r="G262" s="0"/>
-      <c r="H262" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="I262" s="0"/>
+        <v>0</v>
+      </c>
+      <c r="B262" t="n" s="0">
+        <v>48.0</v>
+      </c>
     </row>
     <row r="263">
-      <c r="A263" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B263" t="n" s="0">
-        <v>48.0</v>
+      <c r="A263" t="n" s="1">
+        <v>45985.0</v>
+      </c>
+      <c r="B263" t="s" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="264">
-      <c r="A264" t="n" s="1">
-        <v>45985.0</v>
-      </c>
-      <c r="B264" t="s" s="0">
-        <v>1</v>
-      </c>
+      <c r="A264" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="B264" s="0"/>
+      <c r="C264" s="0"/>
+      <c r="D264" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E264" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F264" s="0"/>
+      <c r="G264" s="0"/>
+      <c r="H264" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="I264" s="0"/>
     </row>
     <row r="265">
       <c r="A265" t="s" s="0">
@@ -5434,10 +5445,10 @@
       <c r="B265" s="0"/>
       <c r="C265" s="0"/>
       <c r="D265" t="s" s="0">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E265" t="n" s="0">
-        <v>2.0</v>
+        <v>4.0</v>
       </c>
       <c r="F265" s="0"/>
       <c r="G265" s="0"/>
@@ -5447,35 +5458,39 @@
       <c r="I265" s="0"/>
     </row>
     <row r="266">
-      <c r="A266" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="B266" s="0"/>
-      <c r="C266" s="0"/>
-      <c r="D266" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E266" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="F266" s="0"/>
-      <c r="G266" s="0"/>
-      <c r="H266" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="I266" s="0"/>
+      <c r="A266" t="n" s="1">
+        <v>45986.0</v>
+      </c>
+      <c r="B266" t="s" s="0">
+        <v>18</v>
+      </c>
     </row>
     <row r="267">
-      <c r="A267" t="n" s="1">
-        <v>45986.0</v>
+      <c r="A267" t="s" s="0">
+        <v>87</v>
       </c>
       <c r="B267" t="s" s="0">
-        <v>18</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="C267" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="D267" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E267" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F267" s="0"/>
+      <c r="G267" s="0"/>
+      <c r="H267" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="I267" s="0"/>
     </row>
     <row r="268">
       <c r="A268" t="s" s="0">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B268" t="s" s="0">
         <v>88</v>
@@ -5484,7 +5499,7 @@
         <v>89</v>
       </c>
       <c r="D268" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E268" t="n" s="0">
         <v>2.0</v>
@@ -5492,57 +5507,57 @@
       <c r="F268" s="0"/>
       <c r="G268" s="0"/>
       <c r="H268" t="s" s="0">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="I268" s="0"/>
     </row>
     <row r="269">
-      <c r="A269" t="s" s="0">
-        <v>90</v>
+      <c r="A269" t="n" s="1">
+        <v>45987.0</v>
       </c>
       <c r="B269" t="s" s="0">
-        <v>88</v>
-      </c>
-      <c r="C269" t="s" s="0">
-        <v>89</v>
-      </c>
-      <c r="D269" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E269" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F269" s="0"/>
-      <c r="G269" s="0"/>
-      <c r="H269" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="I269" s="0"/>
+        <v>23</v>
+      </c>
     </row>
     <row r="270">
-      <c r="A270" t="n" s="1">
-        <v>45987.0</v>
-      </c>
-      <c r="B270" t="s" s="0">
-        <v>23</v>
-      </c>
+      <c r="A270" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B270" s="0"/>
+      <c r="C270" s="0"/>
+      <c r="D270" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E270" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="F270" s="0"/>
+      <c r="G270" s="0"/>
+      <c r="H270" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="I270" s="0"/>
     </row>
     <row r="271">
       <c r="A271" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="B271" s="0"/>
-      <c r="C271" s="0"/>
+        <v>44</v>
+      </c>
+      <c r="B271" t="s" s="0">
+        <v>45</v>
+      </c>
+      <c r="C271" t="s" s="0">
+        <v>75</v>
+      </c>
       <c r="D271" t="s" s="0">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E271" t="n" s="0">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="F271" s="0"/>
       <c r="G271" s="0"/>
       <c r="H271" t="s" s="0">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="I271" s="0"/>
     </row>
@@ -5557,7 +5572,7 @@
         <v>75</v>
       </c>
       <c r="D272" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E272" t="n" s="0">
         <v>2.0</v>
@@ -5570,48 +5585,44 @@
       <c r="I272" s="0"/>
     </row>
     <row r="273">
-      <c r="A273" t="s" s="0">
-        <v>44</v>
+      <c r="A273" t="n" s="1">
+        <v>45988.0</v>
       </c>
       <c r="B273" t="s" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="274">
+      <c r="A274" t="s" s="0">
+        <v>91</v>
+      </c>
+      <c r="B274" t="s" s="0">
         <v>45</v>
       </c>
-      <c r="C273" t="s" s="0">
-        <v>75</v>
-      </c>
-      <c r="D273" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E273" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F273" s="0"/>
-      <c r="G273" s="0"/>
-      <c r="H273" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="I273" s="0"/>
-    </row>
-    <row r="274">
-      <c r="A274" t="n" s="1">
-        <v>45988.0</v>
-      </c>
-      <c r="B274" t="s" s="0">
-        <v>27</v>
-      </c>
+      <c r="C274" t="s" s="0">
+        <v>46</v>
+      </c>
+      <c r="D274" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E274" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F274" s="0"/>
+      <c r="G274" s="0"/>
+      <c r="H274" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="I274" s="0"/>
     </row>
     <row r="275">
       <c r="A275" t="s" s="0">
-        <v>91</v>
-      </c>
-      <c r="B275" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="C275" t="s" s="0">
-        <v>46</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B275" s="0"/>
+      <c r="C275" s="0"/>
       <c r="D275" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E275" t="n" s="0">
         <v>2.0</v>
@@ -5619,26 +5630,32 @@
       <c r="F275" s="0"/>
       <c r="G275" s="0"/>
       <c r="H275" t="s" s="0">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="I275" s="0"/>
     </row>
     <row r="276">
       <c r="A276" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="B276" s="0"/>
-      <c r="C276" s="0"/>
+        <v>69</v>
+      </c>
+      <c r="B276" t="s" s="0">
+        <v>21</v>
+      </c>
+      <c r="C276" t="s" s="0">
+        <v>70</v>
+      </c>
       <c r="D276" t="s" s="0">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E276" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F276" s="0"/>
-      <c r="G276" s="0"/>
+      <c r="G276" t="s" s="0">
+        <v>31</v>
+      </c>
       <c r="H276" t="s" s="0">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="I276" s="0"/>
     </row>
@@ -5660,7 +5677,7 @@
       </c>
       <c r="F277" s="0"/>
       <c r="G277" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H277" t="s" s="0">
         <v>32</v>
@@ -5668,50 +5685,48 @@
       <c r="I277" s="0"/>
     </row>
     <row r="278">
-      <c r="A278" t="s" s="0">
-        <v>69</v>
+      <c r="A278" t="n" s="1">
+        <v>45989.0</v>
       </c>
       <c r="B278" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="C278" t="s" s="0">
-        <v>70</v>
-      </c>
-      <c r="D278" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E278" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F278" s="0"/>
-      <c r="G278" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="H278" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="I278" s="0"/>
+        <v>34</v>
+      </c>
     </row>
     <row r="279">
-      <c r="A279" t="n" s="1">
-        <v>45989.0</v>
+      <c r="A279" t="s" s="0">
+        <v>92</v>
       </c>
       <c r="B279" t="s" s="0">
-        <v>34</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C279" t="s" s="0">
+        <v>61</v>
+      </c>
+      <c r="D279" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E279" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F279" s="0"/>
+      <c r="G279" s="0"/>
+      <c r="H279" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="I279" s="0"/>
     </row>
     <row r="280">
       <c r="A280" t="s" s="0">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B280" t="s" s="0">
-        <v>60</v>
+        <v>45</v>
       </c>
       <c r="C280" t="s" s="0">
-        <v>61</v>
+        <v>75</v>
       </c>
       <c r="D280" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E280" t="n" s="0">
         <v>2.0</v>
@@ -5719,7 +5734,7 @@
       <c r="F280" s="0"/>
       <c r="G280" s="0"/>
       <c r="H280" t="s" s="0">
-        <v>10</v>
+        <v>58</v>
       </c>
       <c r="I280" s="0"/>
     </row>
@@ -5734,7 +5749,7 @@
         <v>75</v>
       </c>
       <c r="D281" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E281" t="n" s="0">
         <v>2.0</v>
@@ -5748,42 +5763,42 @@
     </row>
     <row r="282">
       <c r="A282" t="s" s="0">
-        <v>91</v>
-      </c>
-      <c r="B282" t="s" s="0">
-        <v>45</v>
-      </c>
-      <c r="C282" t="s" s="0">
-        <v>75</v>
-      </c>
-      <c r="D282" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E282" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F282" s="0"/>
-      <c r="G282" s="0"/>
-      <c r="H282" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="I282" s="0"/>
+        <v>0</v>
+      </c>
+      <c r="B282" t="n" s="0">
+        <v>49.0</v>
+      </c>
     </row>
     <row r="283">
-      <c r="A283" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B283" t="n" s="0">
-        <v>49.0</v>
+      <c r="A283" t="n" s="1">
+        <v>45992.0</v>
+      </c>
+      <c r="B283" t="s" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="284">
-      <c r="A284" t="n" s="1">
-        <v>45992.0</v>
+      <c r="A284" t="s" s="0">
+        <v>87</v>
       </c>
       <c r="B284" t="s" s="0">
-        <v>1</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="C284" t="s" s="0">
+        <v>89</v>
+      </c>
+      <c r="D284" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E284" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F284" s="0"/>
+      <c r="G284" s="0"/>
+      <c r="H284" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="I284" s="0"/>
     </row>
     <row r="285">
       <c r="A285" t="s" s="0">
@@ -5796,7 +5811,7 @@
         <v>89</v>
       </c>
       <c r="D285" t="s" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E285" t="n" s="0">
         <v>2.0</v>
@@ -5810,16 +5825,16 @@
     </row>
     <row r="286">
       <c r="A286" t="s" s="0">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B286" t="s" s="0">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="C286" t="s" s="0">
-        <v>89</v>
+        <v>65</v>
       </c>
       <c r="D286" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E286" t="n" s="0">
         <v>2.0</v>
@@ -5827,7 +5842,7 @@
       <c r="F286" s="0"/>
       <c r="G286" s="0"/>
       <c r="H286" t="s" s="0">
-        <v>10</v>
+        <v>39</v>
       </c>
       <c r="I286" s="0"/>
     </row>
@@ -5842,7 +5857,7 @@
         <v>65</v>
       </c>
       <c r="D287" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E287" t="n" s="0">
         <v>2.0</v>
@@ -5855,35 +5870,35 @@
       <c r="I287" s="0"/>
     </row>
     <row r="288">
-      <c r="A288" t="s" s="0">
-        <v>86</v>
+      <c r="A288" t="n" s="1">
+        <v>45993.0</v>
       </c>
       <c r="B288" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="C288" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="D288" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E288" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F288" s="0"/>
-      <c r="G288" s="0"/>
-      <c r="H288" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="I288" s="0"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="289">
-      <c r="A289" t="n" s="1">
-        <v>45993.0</v>
+      <c r="A289" t="s" s="0">
+        <v>79</v>
       </c>
       <c r="B289" t="s" s="0">
-        <v>18</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C289" t="s" s="0">
+        <v>82</v>
+      </c>
+      <c r="D289" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E289" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F289" s="0"/>
+      <c r="G289" s="0"/>
+      <c r="H289" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="I289" s="0"/>
     </row>
     <row r="290">
       <c r="A290" t="s" s="0">
@@ -5896,7 +5911,7 @@
         <v>82</v>
       </c>
       <c r="D290" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E290" t="n" s="0">
         <v>2.0</v>
@@ -5909,47 +5924,43 @@
       <c r="I290" s="0"/>
     </row>
     <row r="291">
-      <c r="A291" t="s" s="0">
-        <v>79</v>
+      <c r="A291" t="n" s="1">
+        <v>45994.0</v>
       </c>
       <c r="B291" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C291" t="s" s="0">
-        <v>82</v>
-      </c>
-      <c r="D291" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E291" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F291" s="0"/>
-      <c r="G291" s="0"/>
-      <c r="H291" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="I291" s="0"/>
+        <v>23</v>
+      </c>
     </row>
     <row r="292">
-      <c r="A292" t="n" s="1">
-        <v>45994.0</v>
-      </c>
-      <c r="B292" t="s" s="0">
-        <v>23</v>
-      </c>
+      <c r="A292" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B292" s="0"/>
+      <c r="C292" s="0"/>
+      <c r="D292" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E292" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="F292" s="0"/>
+      <c r="G292" s="0"/>
+      <c r="H292" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="I292" s="0"/>
     </row>
     <row r="293">
       <c r="A293" t="s" s="0">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="B293" s="0"/>
       <c r="C293" s="0"/>
       <c r="D293" t="s" s="0">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E293" t="n" s="0">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="F293" s="0"/>
       <c r="G293" s="0"/>
@@ -5960,66 +5971,70 @@
     </row>
     <row r="294">
       <c r="A294" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="B294" s="0"/>
-      <c r="C294" s="0"/>
+        <v>86</v>
+      </c>
+      <c r="B294" t="s" s="0">
+        <v>53</v>
+      </c>
+      <c r="C294" t="s" s="0">
+        <v>65</v>
+      </c>
       <c r="D294" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E294" t="n" s="0">
-        <v>2.0</v>
+        <v>3.0</v>
       </c>
       <c r="F294" s="0"/>
       <c r="G294" s="0"/>
       <c r="H294" t="s" s="0">
-        <v>5</v>
+        <v>39</v>
       </c>
       <c r="I294" s="0"/>
     </row>
     <row r="295">
-      <c r="A295" t="s" s="0">
-        <v>86</v>
+      <c r="A295" t="n" s="1">
+        <v>45995.0</v>
       </c>
       <c r="B295" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="C295" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="D295" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E295" t="n" s="0">
-        <v>3.0</v>
-      </c>
-      <c r="F295" s="0"/>
-      <c r="G295" s="0"/>
-      <c r="H295" t="s" s="0">
-        <v>39</v>
-      </c>
-      <c r="I295" s="0"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="296">
-      <c r="A296" t="n" s="1">
-        <v>45995.0</v>
+      <c r="A296" t="s" s="0">
+        <v>93</v>
       </c>
       <c r="B296" t="s" s="0">
-        <v>27</v>
-      </c>
+        <v>21</v>
+      </c>
+      <c r="C296" t="s" s="0">
+        <v>3</v>
+      </c>
+      <c r="D296" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E296" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F296" s="0"/>
+      <c r="G296" s="0"/>
+      <c r="H296" t="s" s="0">
+        <v>58</v>
+      </c>
+      <c r="I296" s="0"/>
     </row>
     <row r="297">
       <c r="A297" t="s" s="0">
-        <v>93</v>
+        <v>87</v>
       </c>
       <c r="B297" t="s" s="0">
-        <v>21</v>
+        <v>88</v>
       </c>
       <c r="C297" t="s" s="0">
-        <v>3</v>
+        <v>54</v>
       </c>
       <c r="D297" t="s" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E297" t="n" s="0">
         <v>2.0</v>
@@ -6027,13 +6042,13 @@
       <c r="F297" s="0"/>
       <c r="G297" s="0"/>
       <c r="H297" t="s" s="0">
-        <v>58</v>
+        <v>10</v>
       </c>
       <c r="I297" s="0"/>
     </row>
     <row r="298">
       <c r="A298" t="s" s="0">
-        <v>87</v>
+        <v>94</v>
       </c>
       <c r="B298" t="s" s="0">
         <v>88</v>
@@ -6042,15 +6057,17 @@
         <v>54</v>
       </c>
       <c r="D298" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E298" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F298" s="0"/>
-      <c r="G298" s="0"/>
+      <c r="G298" t="s" s="0">
+        <v>31</v>
+      </c>
       <c r="H298" t="s" s="0">
-        <v>10</v>
+        <v>32</v>
       </c>
       <c r="I298" s="0"/>
     </row>
@@ -6072,7 +6089,7 @@
       </c>
       <c r="F299" s="0"/>
       <c r="G299" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H299" t="s" s="0">
         <v>32</v>
@@ -6081,45 +6098,45 @@
     </row>
     <row r="300">
       <c r="A300" t="s" s="0">
-        <v>94</v>
-      </c>
-      <c r="B300" t="s" s="0">
-        <v>88</v>
-      </c>
-      <c r="C300" t="s" s="0">
-        <v>54</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B300" s="0"/>
+      <c r="C300" s="0"/>
       <c r="D300" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E300" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F300" s="0"/>
-      <c r="G300" t="s" s="0">
-        <v>33</v>
-      </c>
+      <c r="G300" s="0"/>
       <c r="H300" t="s" s="0">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="I300" s="0"/>
     </row>
     <row r="301">
       <c r="A301" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="B301" s="0"/>
-      <c r="C301" s="0"/>
+        <v>94</v>
+      </c>
+      <c r="B301" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="C301" t="s" s="0">
+        <v>54</v>
+      </c>
       <c r="D301" t="s" s="0">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E301" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F301" s="0"/>
-      <c r="G301" s="0"/>
+      <c r="G301" t="s" s="0">
+        <v>31</v>
+      </c>
       <c r="H301" t="s" s="0">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="I301" s="0"/>
     </row>
@@ -6141,7 +6158,7 @@
       </c>
       <c r="F302" s="0"/>
       <c r="G302" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H302" t="s" s="0">
         <v>32</v>
@@ -6149,72 +6166,72 @@
       <c r="I302" s="0"/>
     </row>
     <row r="303">
-      <c r="A303" t="s" s="0">
-        <v>94</v>
+      <c r="A303" t="n" s="1">
+        <v>45996.0</v>
       </c>
       <c r="B303" t="s" s="0">
-        <v>88</v>
-      </c>
-      <c r="C303" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="D303" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E303" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F303" s="0"/>
-      <c r="G303" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="H303" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="I303" s="0"/>
+        <v>34</v>
+      </c>
     </row>
     <row r="304">
-      <c r="A304" t="n" s="1">
-        <v>45996.0</v>
-      </c>
-      <c r="B304" t="s" s="0">
-        <v>34</v>
-      </c>
+      <c r="A304" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="B304" s="0"/>
+      <c r="C304" s="0"/>
+      <c r="D304" t="s" s="0">
+        <v>14</v>
+      </c>
+      <c r="E304" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="F304" s="0"/>
+      <c r="G304" s="0"/>
+      <c r="H304" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="I304" s="0"/>
     </row>
     <row r="305">
       <c r="A305" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="B305" s="0"/>
-      <c r="C305" s="0"/>
-      <c r="D305" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E305" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="F305" s="0"/>
-      <c r="G305" s="0"/>
-      <c r="H305" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="I305" s="0"/>
+        <v>0</v>
+      </c>
+      <c r="B305" t="n" s="0">
+        <v>50.0</v>
+      </c>
     </row>
     <row r="306">
-      <c r="A306" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B306" t="n" s="0">
-        <v>50.0</v>
+      <c r="A306" t="n" s="1">
+        <v>45999.0</v>
+      </c>
+      <c r="B306" t="s" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="307">
-      <c r="A307" t="n" s="1">
-        <v>45999.0</v>
+      <c r="A307" t="s" s="0">
+        <v>48</v>
       </c>
       <c r="B307" t="s" s="0">
-        <v>1</v>
-      </c>
+        <v>7</v>
+      </c>
+      <c r="C307" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D307" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E307" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F307" s="0"/>
+      <c r="G307" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="H307" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="I307" s="0"/>
     </row>
     <row r="308">
       <c r="A308" t="s" s="0">
@@ -6227,14 +6244,14 @@
         <v>8</v>
       </c>
       <c r="D308" t="s" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E308" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F308" s="0"/>
       <c r="G308" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H308" t="s" s="0">
         <v>32</v>
@@ -6243,23 +6260,21 @@
     </row>
     <row r="309">
       <c r="A309" t="s" s="0">
-        <v>48</v>
+        <v>95</v>
       </c>
       <c r="B309" t="s" s="0">
         <v>7</v>
       </c>
-      <c r="C309" t="s" s="0">
-        <v>8</v>
-      </c>
+      <c r="C309" s="0"/>
       <c r="D309" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E309" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F309" s="0"/>
       <c r="G309" t="s" s="0">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H309" t="s" s="0">
         <v>32</v>
@@ -6268,195 +6283,195 @@
     </row>
     <row r="310">
       <c r="A310" t="s" s="0">
-        <v>95</v>
-      </c>
-      <c r="B310" t="s" s="0">
-        <v>7</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B310" s="0"/>
       <c r="C310" s="0"/>
       <c r="D310" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E310" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F310" s="0"/>
-      <c r="G310" t="s" s="0">
-        <v>31</v>
-      </c>
+      <c r="G310" s="0"/>
       <c r="H310" t="s" s="0">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="I310" s="0"/>
     </row>
     <row r="311">
       <c r="A311" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="B311" s="0"/>
+        <v>95</v>
+      </c>
+      <c r="B311" t="s" s="0">
+        <v>7</v>
+      </c>
       <c r="C311" s="0"/>
       <c r="D311" t="s" s="0">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E311" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F311" s="0"/>
-      <c r="G311" s="0"/>
+      <c r="G311" t="s" s="0">
+        <v>33</v>
+      </c>
       <c r="H311" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="I311" s="0"/>
+    </row>
+    <row r="312">
+      <c r="A312" t="n" s="1">
+        <v>46000.0</v>
+      </c>
+      <c r="B312" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="313">
+      <c r="A313" t="s" s="0">
+        <v>78</v>
+      </c>
+      <c r="B313" s="0"/>
+      <c r="C313" s="0"/>
+      <c r="D313" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E313" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F313" s="0"/>
+      <c r="G313" s="0"/>
+      <c r="H313" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="I311" s="0"/>
-    </row>
-    <row r="312">
-      <c r="A312" t="s" s="0">
-        <v>95</v>
-      </c>
-      <c r="B312" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C312" s="0"/>
-      <c r="D312" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E312" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F312" s="0"/>
-      <c r="G312" t="s" s="0">
-        <v>33</v>
-      </c>
-      <c r="H312" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="I312" s="0"/>
-    </row>
-    <row r="313">
-      <c r="A313" t="n" s="1">
-        <v>46000.0</v>
-      </c>
-      <c r="B313" t="s" s="0">
-        <v>18</v>
-      </c>
+      <c r="I313" s="0"/>
     </row>
     <row r="314">
       <c r="A314" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="B314" s="0"/>
+        <v>95</v>
+      </c>
+      <c r="B314" t="s" s="0">
+        <v>7</v>
+      </c>
       <c r="C314" s="0"/>
       <c r="D314" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E314" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F314" s="0"/>
-      <c r="G314" s="0"/>
+      <c r="G314" t="s" s="0">
+        <v>33</v>
+      </c>
       <c r="H314" t="s" s="0">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="I314" s="0"/>
     </row>
     <row r="315">
       <c r="A315" t="s" s="0">
-        <v>95</v>
-      </c>
-      <c r="B315" t="s" s="0">
-        <v>7</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B315" s="0"/>
       <c r="C315" s="0"/>
       <c r="D315" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E315" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F315" s="0"/>
-      <c r="G315" t="s" s="0">
-        <v>33</v>
-      </c>
+      <c r="G315" s="0"/>
       <c r="H315" t="s" s="0">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="I315" s="0"/>
     </row>
     <row r="316">
       <c r="A316" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="B316" s="0"/>
+        <v>95</v>
+      </c>
+      <c r="B316" t="s" s="0">
+        <v>7</v>
+      </c>
       <c r="C316" s="0"/>
       <c r="D316" t="s" s="0">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E316" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F316" s="0"/>
-      <c r="G316" s="0"/>
+      <c r="G316" t="s" s="0">
+        <v>31</v>
+      </c>
       <c r="H316" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="I316" s="0"/>
+    </row>
+    <row r="317">
+      <c r="A317" t="n" s="1">
+        <v>46001.0</v>
+      </c>
+      <c r="B317" t="s" s="0">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="318">
+      <c r="A318" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B318" s="0"/>
+      <c r="C318" s="0"/>
+      <c r="D318" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E318" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="F318" s="0"/>
+      <c r="G318" s="0"/>
+      <c r="H318" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="I316" s="0"/>
-    </row>
-    <row r="317">
-      <c r="A317" t="s" s="0">
-        <v>95</v>
-      </c>
-      <c r="B317" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C317" s="0"/>
-      <c r="D317" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E317" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F317" s="0"/>
-      <c r="G317" t="s" s="0">
-        <v>31</v>
-      </c>
-      <c r="H317" t="s" s="0">
-        <v>32</v>
-      </c>
-      <c r="I317" s="0"/>
-    </row>
-    <row r="318">
-      <c r="A318" t="n" s="1">
-        <v>46001.0</v>
-      </c>
-      <c r="B318" t="s" s="0">
-        <v>23</v>
-      </c>
+      <c r="I318" s="0"/>
     </row>
     <row r="319">
-      <c r="A319" t="s" s="0">
-        <v>43</v>
-      </c>
-      <c r="B319" s="0"/>
-      <c r="C319" s="0"/>
-      <c r="D319" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="E319" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="F319" s="0"/>
-      <c r="G319" s="0"/>
-      <c r="H319" t="s" s="0">
-        <v>5</v>
-      </c>
-      <c r="I319" s="0"/>
+      <c r="A319" t="n" s="1">
+        <v>46002.0</v>
+      </c>
+      <c r="B319" t="s" s="0">
+        <v>27</v>
+      </c>
     </row>
     <row r="320">
-      <c r="A320" t="n" s="1">
-        <v>46002.0</v>
+      <c r="A320" t="s" s="0">
+        <v>87</v>
       </c>
       <c r="B320" t="s" s="0">
-        <v>27</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="C320" t="s" s="0">
+        <v>54</v>
+      </c>
+      <c r="D320" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E320" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F320" s="0"/>
+      <c r="G320" s="0"/>
+      <c r="H320" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="I320" s="0"/>
     </row>
     <row r="321">
       <c r="A321" t="s" s="0">
@@ -6469,7 +6484,7 @@
         <v>54</v>
       </c>
       <c r="D321" t="s" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E321" t="n" s="0">
         <v>2.0</v>
@@ -6492,7 +6507,7 @@
         <v>54</v>
       </c>
       <c r="D322" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E322" t="n" s="0">
         <v>2.0</v>
@@ -6505,35 +6520,35 @@
       <c r="I322" s="0"/>
     </row>
     <row r="323">
-      <c r="A323" t="s" s="0">
-        <v>87</v>
+      <c r="A323" t="n" s="1">
+        <v>46003.0</v>
       </c>
       <c r="B323" t="s" s="0">
-        <v>88</v>
-      </c>
-      <c r="C323" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="D323" t="s" s="0">
-        <v>14</v>
-      </c>
-      <c r="E323" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F323" s="0"/>
-      <c r="G323" s="0"/>
-      <c r="H323" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="I323" s="0"/>
+        <v>34</v>
+      </c>
     </row>
     <row r="324">
-      <c r="A324" t="n" s="1">
-        <v>46003.0</v>
+      <c r="A324" t="s" s="0">
+        <v>67</v>
       </c>
       <c r="B324" t="s" s="0">
-        <v>34</v>
-      </c>
+        <v>60</v>
+      </c>
+      <c r="C324" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="D324" t="s" s="0">
+        <v>4</v>
+      </c>
+      <c r="E324" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F324" s="0"/>
+      <c r="G324" s="0"/>
+      <c r="H324" t="s" s="0">
+        <v>10</v>
+      </c>
+      <c r="I324" s="0"/>
     </row>
     <row r="325">
       <c r="A325" t="s" s="0">
@@ -6546,7 +6561,7 @@
         <v>68</v>
       </c>
       <c r="D325" t="s" s="0">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="E325" t="n" s="0">
         <v>2.0</v>
@@ -6560,16 +6575,16 @@
     </row>
     <row r="326">
       <c r="A326" t="s" s="0">
-        <v>67</v>
+        <v>15</v>
       </c>
       <c r="B326" t="s" s="0">
-        <v>60</v>
+        <v>16</v>
       </c>
       <c r="C326" t="s" s="0">
-        <v>68</v>
+        <v>13</v>
       </c>
       <c r="D326" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E326" t="n" s="0">
         <v>2.0</v>
@@ -6592,7 +6607,7 @@
         <v>13</v>
       </c>
       <c r="D327" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E327" t="n" s="0">
         <v>2.0</v>
@@ -6606,42 +6621,42 @@
     </row>
     <row r="328">
       <c r="A328" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="B328" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="C328" t="s" s="0">
-        <v>13</v>
-      </c>
-      <c r="D328" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E328" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F328" s="0"/>
-      <c r="G328" s="0"/>
-      <c r="H328" t="s" s="0">
-        <v>10</v>
-      </c>
-      <c r="I328" s="0"/>
+        <v>0</v>
+      </c>
+      <c r="B328" t="n" s="0">
+        <v>51.0</v>
+      </c>
     </row>
     <row r="329">
-      <c r="A329" t="s" s="0">
-        <v>0</v>
-      </c>
-      <c r="B329" t="n" s="0">
-        <v>51.0</v>
+      <c r="A329" t="n" s="1">
+        <v>46006.0</v>
+      </c>
+      <c r="B329" t="s" s="0">
+        <v>1</v>
       </c>
     </row>
     <row r="330">
-      <c r="A330" t="n" s="1">
-        <v>46006.0</v>
+      <c r="A330" t="s" s="0">
+        <v>96</v>
       </c>
       <c r="B330" t="s" s="0">
-        <v>1</v>
-      </c>
+        <v>88</v>
+      </c>
+      <c r="C330" s="0"/>
+      <c r="D330" t="s" s="0">
+        <v>9</v>
+      </c>
+      <c r="E330" t="n" s="0">
+        <v>2.0</v>
+      </c>
+      <c r="F330" s="0"/>
+      <c r="G330" t="s" s="0">
+        <v>31</v>
+      </c>
+      <c r="H330" t="s" s="0">
+        <v>32</v>
+      </c>
+      <c r="I330" s="0"/>
     </row>
     <row r="331">
       <c r="A331" t="s" s="0">
@@ -6659,7 +6674,7 @@
       </c>
       <c r="F331" s="0"/>
       <c r="G331" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H331" t="s" s="0">
         <v>32</v>
@@ -6668,21 +6683,23 @@
     </row>
     <row r="332">
       <c r="A332" t="s" s="0">
-        <v>96</v>
+        <v>69</v>
       </c>
       <c r="B332" t="s" s="0">
-        <v>88</v>
-      </c>
-      <c r="C332" s="0"/>
+        <v>21</v>
+      </c>
+      <c r="C332" t="s" s="0">
+        <v>70</v>
+      </c>
       <c r="D332" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E332" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F332" s="0"/>
       <c r="G332" t="s" s="0">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="H332" t="s" s="0">
         <v>32</v>
@@ -6700,14 +6717,14 @@
         <v>70</v>
       </c>
       <c r="D333" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E333" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F333" s="0"/>
       <c r="G333" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H333" t="s" s="0">
         <v>32</v>
@@ -6716,72 +6733,72 @@
     </row>
     <row r="334">
       <c r="A334" t="s" s="0">
-        <v>69</v>
-      </c>
-      <c r="B334" t="s" s="0">
-        <v>21</v>
-      </c>
-      <c r="C334" t="s" s="0">
-        <v>70</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B334" s="0"/>
+      <c r="C334" s="0"/>
       <c r="D334" t="s" s="0">
-        <v>17</v>
+        <v>30</v>
       </c>
       <c r="E334" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F334" s="0"/>
-      <c r="G334" t="s" s="0">
-        <v>33</v>
-      </c>
+      <c r="G334" s="0"/>
       <c r="H334" t="s" s="0">
-        <v>32</v>
+        <v>5</v>
       </c>
       <c r="I334" s="0"/>
     </row>
     <row r="335">
-      <c r="A335" t="s" s="0">
+      <c r="A335" t="n" s="1">
+        <v>46007.0</v>
+      </c>
+      <c r="B335" t="s" s="0">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="336">
+      <c r="A336" t="s" s="0">
         <v>78</v>
       </c>
-      <c r="B335" s="0"/>
-      <c r="C335" s="0"/>
-      <c r="D335" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E335" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F335" s="0"/>
-      <c r="G335" s="0"/>
-      <c r="H335" t="s" s="0">
+      <c r="B336" s="0"/>
+      <c r="C336" s="0"/>
+      <c r="D336" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E336" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="F336" s="0"/>
+      <c r="G336" s="0"/>
+      <c r="H336" t="s" s="0">
         <v>5</v>
       </c>
-      <c r="I335" s="0"/>
-    </row>
-    <row r="336">
-      <c r="A336" t="n" s="1">
-        <v>46007.0</v>
-      </c>
-      <c r="B336" t="s" s="0">
-        <v>18</v>
-      </c>
+      <c r="I336" s="0"/>
     </row>
     <row r="337">
       <c r="A337" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="B337" s="0"/>
-      <c r="C337" s="0"/>
+        <v>97</v>
+      </c>
+      <c r="B337" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="C337" t="s" s="0">
+        <v>89</v>
+      </c>
       <c r="D337" t="s" s="0">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E337" t="n" s="0">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="F337" s="0"/>
-      <c r="G337" s="0"/>
+      <c r="G337" t="s" s="0">
+        <v>31</v>
+      </c>
       <c r="H337" t="s" s="0">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="I337" s="0"/>
     </row>
@@ -6803,7 +6820,7 @@
       </c>
       <c r="F338" s="0"/>
       <c r="G338" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H338" t="s" s="0">
         <v>32</v>
@@ -6812,71 +6829,65 @@
     </row>
     <row r="339">
       <c r="A339" t="s" s="0">
-        <v>97</v>
+        <v>52</v>
       </c>
       <c r="B339" t="s" s="0">
-        <v>88</v>
+        <v>53</v>
       </c>
       <c r="C339" t="s" s="0">
-        <v>89</v>
+        <v>54</v>
       </c>
       <c r="D339" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E339" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F339" s="0"/>
-      <c r="G339" t="s" s="0">
-        <v>33</v>
-      </c>
+      <c r="G339" s="0"/>
       <c r="H339" t="s" s="0">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="I339" s="0"/>
     </row>
     <row r="340">
-      <c r="A340" t="s" s="0">
-        <v>52</v>
+      <c r="A340" t="n" s="1">
+        <v>46008.0</v>
       </c>
       <c r="B340" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="C340" t="s" s="0">
-        <v>54</v>
-      </c>
-      <c r="D340" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E340" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F340" s="0"/>
-      <c r="G340" s="0"/>
-      <c r="H340" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="I340" s="0"/>
+        <v>23</v>
+      </c>
     </row>
     <row r="341">
-      <c r="A341" t="n" s="1">
-        <v>46008.0</v>
-      </c>
-      <c r="B341" t="s" s="0">
-        <v>23</v>
-      </c>
+      <c r="A341" t="s" s="0">
+        <v>43</v>
+      </c>
+      <c r="B341" s="0"/>
+      <c r="C341" s="0"/>
+      <c r="D341" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E341" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="F341" s="0"/>
+      <c r="G341" s="0"/>
+      <c r="H341" t="s" s="0">
+        <v>5</v>
+      </c>
+      <c r="I341" s="0"/>
     </row>
     <row r="342">
       <c r="A342" t="s" s="0">
-        <v>43</v>
+        <v>78</v>
       </c>
       <c r="B342" s="0"/>
       <c r="C342" s="0"/>
       <c r="D342" t="s" s="0">
-        <v>25</v>
+        <v>14</v>
       </c>
       <c r="E342" t="n" s="0">
-        <v>4.0</v>
+        <v>2.0</v>
       </c>
       <c r="F342" s="0"/>
       <c r="G342" s="0"/>
@@ -6887,42 +6898,46 @@
     </row>
     <row r="343">
       <c r="A343" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="B343" s="0"/>
-      <c r="C343" s="0"/>
+        <v>98</v>
+      </c>
+      <c r="B343" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C343" t="s" s="0">
+        <v>99</v>
+      </c>
       <c r="D343" t="s" s="0">
-        <v>14</v>
+        <v>100</v>
       </c>
       <c r="E343" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F343" s="0"/>
+        <v>1.0</v>
+      </c>
+      <c r="F343" t="s" s="0">
+        <v>65</v>
+      </c>
       <c r="G343" s="0"/>
       <c r="H343" t="s" s="0">
-        <v>5</v>
+        <v>58</v>
       </c>
       <c r="I343" s="0"/>
     </row>
     <row r="344">
       <c r="A344" t="s" s="0">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="B344" t="s" s="0">
-        <v>7</v>
+        <v>53</v>
       </c>
       <c r="C344" t="s" s="0">
-        <v>99</v>
+        <v>65</v>
       </c>
       <c r="D344" t="s" s="0">
-        <v>100</v>
+        <v>30</v>
       </c>
       <c r="E344" t="n" s="0">
         <v>1.0</v>
       </c>
-      <c r="F344" t="s" s="0">
-        <v>65</v>
-      </c>
+      <c r="F344" s="0"/>
       <c r="G344" s="0"/>
       <c r="H344" t="s" s="0">
         <v>58</v>
@@ -6930,75 +6945,77 @@
       <c r="I344" s="0"/>
     </row>
     <row r="345">
-      <c r="A345" t="s" s="0">
-        <v>101</v>
+      <c r="A345" t="n" s="1">
+        <v>46009.0</v>
       </c>
       <c r="B345" t="s" s="0">
-        <v>53</v>
-      </c>
-      <c r="C345" t="s" s="0">
-        <v>65</v>
-      </c>
-      <c r="D345" t="s" s="0">
-        <v>30</v>
-      </c>
-      <c r="E345" t="n" s="0">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="346">
+      <c r="A346" t="s" s="0">
+        <v>102</v>
+      </c>
+      <c r="B346" t="s" s="0">
+        <v>60</v>
+      </c>
+      <c r="C346" t="s" s="0">
+        <v>68</v>
+      </c>
+      <c r="D346" t="s" s="0">
+        <v>103</v>
+      </c>
+      <c r="E346" t="n" s="0">
         <v>1.0</v>
       </c>
-      <c r="F345" s="0"/>
-      <c r="G345" s="0"/>
-      <c r="H345" t="s" s="0">
+      <c r="F346" s="0"/>
+      <c r="G346" s="0"/>
+      <c r="H346" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="I345" s="0"/>
-    </row>
-    <row r="346">
-      <c r="A346" t="n" s="1">
-        <v>46009.0</v>
-      </c>
-      <c r="B346" t="s" s="0">
-        <v>27</v>
-      </c>
+      <c r="I346" s="0"/>
     </row>
     <row r="347">
       <c r="A347" t="s" s="0">
-        <v>102</v>
-      </c>
-      <c r="B347" t="s" s="0">
-        <v>60</v>
-      </c>
-      <c r="C347" t="s" s="0">
-        <v>68</v>
-      </c>
+        <v>78</v>
+      </c>
+      <c r="B347" s="0"/>
+      <c r="C347" s="0"/>
       <c r="D347" t="s" s="0">
-        <v>103</v>
+        <v>9</v>
       </c>
       <c r="E347" t="n" s="0">
-        <v>1.0</v>
+        <v>2.0</v>
       </c>
       <c r="F347" s="0"/>
       <c r="G347" s="0"/>
       <c r="H347" t="s" s="0">
-        <v>58</v>
+        <v>5</v>
       </c>
       <c r="I347" s="0"/>
     </row>
     <row r="348">
       <c r="A348" t="s" s="0">
-        <v>78</v>
-      </c>
-      <c r="B348" s="0"/>
-      <c r="C348" s="0"/>
+        <v>97</v>
+      </c>
+      <c r="B348" t="s" s="0">
+        <v>88</v>
+      </c>
+      <c r="C348" t="s" s="0">
+        <v>89</v>
+      </c>
       <c r="D348" t="s" s="0">
-        <v>9</v>
+        <v>14</v>
       </c>
       <c r="E348" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F348" s="0"/>
-      <c r="G348" s="0"/>
+      <c r="G348" t="s" s="0">
+        <v>31</v>
+      </c>
       <c r="H348" t="s" s="0">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="I348" s="0"/>
     </row>
@@ -7020,7 +7037,7 @@
       </c>
       <c r="F349" s="0"/>
       <c r="G349" t="s" s="0">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="H349" t="s" s="0">
         <v>32</v>
@@ -7029,82 +7046,57 @@
     </row>
     <row r="350">
       <c r="A350" t="s" s="0">
-        <v>97</v>
+        <v>104</v>
       </c>
       <c r="B350" t="s" s="0">
         <v>88</v>
       </c>
       <c r="C350" t="s" s="0">
-        <v>89</v>
+        <v>105</v>
       </c>
       <c r="D350" t="s" s="0">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="E350" t="n" s="0">
         <v>2.0</v>
       </c>
       <c r="F350" s="0"/>
-      <c r="G350" t="s" s="0">
-        <v>33</v>
-      </c>
+      <c r="G350" s="0"/>
       <c r="H350" t="s" s="0">
-        <v>32</v>
+        <v>58</v>
       </c>
       <c r="I350" s="0"/>
     </row>
     <row r="351">
-      <c r="A351" t="s" s="0">
-        <v>104</v>
+      <c r="A351" t="n" s="1">
+        <v>46010.0</v>
       </c>
       <c r="B351" t="s" s="0">
-        <v>88</v>
-      </c>
-      <c r="C351" t="s" s="0">
-        <v>105</v>
-      </c>
-      <c r="D351" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="E351" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F351" s="0"/>
-      <c r="G351" s="0"/>
-      <c r="H351" t="s" s="0">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="352">
+      <c r="A352" t="s" s="0">
+        <v>106</v>
+      </c>
+      <c r="B352" t="s" s="0">
+        <v>7</v>
+      </c>
+      <c r="C352" t="s" s="0">
+        <v>8</v>
+      </c>
+      <c r="D352" t="s" s="0">
+        <v>25</v>
+      </c>
+      <c r="E352" t="n" s="0">
+        <v>4.0</v>
+      </c>
+      <c r="F352" s="0"/>
+      <c r="G352" s="0"/>
+      <c r="H352" t="s" s="0">
         <v>58</v>
       </c>
-      <c r="I351" s="0"/>
-    </row>
-    <row r="352">
-      <c r="A352" t="n" s="1">
-        <v>46010.0</v>
-      </c>
-      <c r="B352" t="s" s="0">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="353">
-      <c r="A353" t="s" s="0">
-        <v>106</v>
-      </c>
-      <c r="B353" t="s" s="0">
-        <v>7</v>
-      </c>
-      <c r="C353" t="s" s="0">
-        <v>8</v>
-      </c>
-      <c r="D353" t="s" s="0">
-        <v>25</v>
-      </c>
-      <c r="E353" t="n" s="0">
-        <v>4.0</v>
-      </c>
-      <c r="F353" s="0"/>
-      <c r="G353" s="0"/>
-      <c r="H353" t="s" s="0">
-        <v>58</v>
-      </c>
-      <c r="I353" s="0"/>
+      <c r="I352" s="0"/>
     </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>

</xml_diff>